<commit_message>
Update(Plannification) : Ajout de ma plannification du  Mardi 28 Octobre
</commit_message>
<xml_diff>
--- a/Plannification_VicheryAaron.xlsx
+++ b/Plannification_VicheryAaron.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2eme\Modules\Module 320\Projet\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C0248-79E2-4D70-93B7-4BD7390D9631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022CA7BD-00FA-46CF-B330-AABB712A5636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Je vais faire le journal de travail de ce que j'ai fait aujourd'hui</t>
+  </si>
+  <si>
+    <t>Je vais ajouter les obstacles dans mon jeu</t>
+  </si>
+  <si>
+    <t>Je vais essayer de faire déplacer les obstacles et les ennemis en même temps</t>
+  </si>
+  <si>
+    <t>Je vais ajouter les collisions dans mon jeu</t>
+  </si>
+  <si>
+    <t>J'avais oublié de faire la plannification pour la semaine avant les vacances et le lundi 27 octobre</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1180,7 @@
                   <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>190</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2020,16 +2032,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.32098765432098764</c:v>
+                  <c:v>0.20634920634920634</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46913580246913578</c:v>
+                  <c:v>0.65873015873015872</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20987654320987653</c:v>
+                  <c:v>0.13492063492063491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4213,9 +4225,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4268,7 +4280,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 45 minutes</v>
+        <v>10 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4281,15 +4293,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>405</v>
+        <v>630</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4616,7 +4628,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="str">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
         <v/>
@@ -4626,48 +4638,76 @@
       <c r="D18" s="32"/>
       <c r="E18" s="33"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="39"/>
+      <c r="G18" s="39" t="s">
+        <v>42</v>
+      </c>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45958</v>
+      </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>30</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45958</v>
+      </c>
+      <c r="C20" s="31">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>15</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+        <v>44</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45958</v>
+      </c>
+      <c r="C21" s="35">
+        <v>2</v>
+      </c>
       <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
+      <c r="E21" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -10961,7 +11001,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.32098765432098764</v>
+        <v>0.20634920634920634</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10978,15 +11018,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>415</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10994,11 +11034,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>3 h 10 min</v>
+        <v>6 h 55 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.46913580246913578</v>
+        <v>0.65873015873015872</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11072,7 +11112,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.20987654320987653</v>
+        <v>0.13492063492063491</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11124,26 +11164,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>405</v>
+        <v>630</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 45 min</v>
+        <v>10 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11187,20 +11227,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8ff2034f-5386-4151-8c46-54da7a5b32f0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8ff2034f-5386-4151-8c46-54da7a5b32f0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11392,14 +11432,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="8ff2034f-5386-4151-8c46-54da7a5b32f0"/>
@@ -11411,6 +11443,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update(Plannification) : Ajout de ma plannification du mercredi 29 octobre
</commit_message>
<xml_diff>
--- a/Plannification_VicheryAaron.xlsx
+++ b/Plannification_VicheryAaron.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022CA7BD-00FA-46CF-B330-AABB712A5636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A798C0-4513-46F1-9F83-720CFBD78092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>J'avais oublié de faire la plannification pour la semaine avant les vacances et le lundi 27 octobre</t>
+  </si>
+  <si>
+    <t>Je vais faire tous les commentaires de mon code</t>
+  </si>
+  <si>
+    <t>Je vais essayer d'ajouter les collisions dans mon jeu</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1186,7 @@
                   <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>415</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1253,7 +1259,6 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1261,6 +1266,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1600,7 +1606,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1608,6 +1613,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2032,16 +2038,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.20634920634920634</c:v>
+                  <c:v>0.17687074829931973</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65873015873015872</c:v>
+                  <c:v>0.70748299319727892</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13492063492063491</c:v>
+                  <c:v>0.11564625850340136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2196,7 +2202,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2204,6 +2209,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4225,9 +4231,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4280,7 +4286,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>10 heures 30 minutes</v>
+        <v>12 heures 15 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4293,15 +4299,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>630</v>
+        <v>735</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4711,27 +4717,45 @@
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45959</v>
+      </c>
       <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="23"/>
+      <c r="D22" s="32">
+        <v>15</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="str">
+      <c r="A23" s="63">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B23" s="34">
+        <v>45959</v>
+      </c>
+      <c r="C23" s="35">
+        <v>1</v>
+      </c>
+      <c r="D23" s="36">
+        <v>30</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -11001,7 +11025,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.20634920634920634</v>
+        <v>0.17687074829931973</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11018,15 +11042,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>415</v>
+        <v>520</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11034,11 +11058,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>6 h 55 min</v>
+        <v>8 h 40 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.65873015873015872</v>
+        <v>0.70748299319727892</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11112,7 +11136,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.13492063492063491</v>
+        <v>0.11564625850340136</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11164,26 +11188,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>630</v>
+        <v>735</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>10 h 30 min</v>
+        <v>12 h 15 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.11666666666666667</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11227,20 +11251,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8ff2034f-5386-4151-8c46-54da7a5b32f0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8ff2034f-5386-4151-8c46-54da7a5b32f0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11432,6 +11456,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="8ff2034f-5386-4151-8c46-54da7a5b32f0"/>
@@ -11443,14 +11475,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update(Rapport): Rajouter la plannification d'avancement du rapport
</commit_message>
<xml_diff>
--- a/Plannification_VicheryAaron.xlsx
+++ b/Plannification_VicheryAaron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A798C0-4513-46F1-9F83-720CFBD78092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20861A37-3F5A-471E-AE6C-FE08011FD125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Je vais essayer d'ajouter les collisions dans mon jeu</t>
+  </si>
+  <si>
+    <t>Je vais continuer mon rapport</t>
   </si>
 </sst>
 </file>
@@ -1186,13 +1189,13 @@
                   <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>520</c:v>
+                  <c:v>535</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2038,16 +2041,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.17687074829931973</c:v>
+                  <c:v>0.16352201257861634</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70748299319727892</c:v>
+                  <c:v>0.67295597484276726</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11564625850340136</c:v>
+                  <c:v>0.16352201257861634</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4233,7 +4236,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4286,7 +4289,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>12 heures 15 minutes</v>
+        <v>13 heures 15 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4303,11 +4306,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>315</v>
+        <v>375</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>735</v>
+        <v>795</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4726,7 +4729,7 @@
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="32">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E22" s="33" t="s">
         <v>16</v>
@@ -4759,15 +4762,23 @@
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="str">
+      <c r="A24" s="62">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B24" s="30">
+        <v>45959</v>
+      </c>
       <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="23"/>
+      <c r="D24" s="32">
+        <v>45</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -11025,7 +11036,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.17687074829931973</v>
+        <v>0.16352201257861634</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11046,11 +11057,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>520</v>
+        <v>535</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11058,11 +11069,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>8 h 40 min</v>
+        <v>8 h 55 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.70748299319727892</v>
+        <v>0.67295597484276726</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11120,11 +11131,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11132,11 +11143,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 25 min</v>
+        <v>2 h 10 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.11564625850340136</v>
+        <v>0.16352201257861634</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11192,22 +11203,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>315</v>
+        <v>375</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>735</v>
+        <v>795</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>12 h 15 min</v>
+        <v>13 h 15 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.1361111111111111</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update(Plannification) : Ajout de la plannification de ce que je vais faire aujourd'hui
</commit_message>
<xml_diff>
--- a/Plannification_VicheryAaron.xlsx
+++ b/Plannification_VicheryAaron.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_OO-320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20861A37-3F5A-471E-AE6C-FE08011FD125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B070E3-01E3-45F6-9CF8-3A1D6CD45A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>Je vais continuer mon rapport</t>
+  </si>
+  <si>
+    <t>Je vais ajouter les commentaires dans mon code</t>
+  </si>
+  <si>
+    <t>Je vais rajouter les maquettes dans mon projet sur github</t>
+  </si>
+  <si>
+    <t>Je vais finir mon rapport</t>
   </si>
 </sst>
 </file>
@@ -1186,16 +1195,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>130</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>535</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1262,6 +1271,7 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1269,7 +1279,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1609,6 +1618,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1616,7 +1626,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2041,16 +2050,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.16352201257861634</c:v>
+                  <c:v>0.17486338797814208</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67295597484276726</c:v>
+                  <c:v>0.61748633879781423</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16352201257861634</c:v>
+                  <c:v>0.20765027322404372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2205,6 +2214,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2212,7 +2222,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4236,7 +4245,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4289,7 +4298,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>13 heures 15 minutes</v>
+        <v>15 heures 15 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4302,15 +4311,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>795</v>
+        <v>915</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4782,39 +4791,65 @@
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="str">
+      <c r="A25" s="63">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B25" s="34">
+        <v>45961</v>
+      </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="23"/>
+      <c r="D25" s="36">
+        <v>30</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="62" t="str">
+      <c r="A26" s="62">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B26" s="30">
+        <v>45961</v>
+      </c>
       <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="23"/>
+      <c r="D26" s="32">
+        <v>30</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="str">
+      <c r="A27" s="63">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="B27" s="34">
+        <v>45961</v>
+      </c>
+      <c r="C27" s="35">
+        <v>1</v>
+      </c>
+      <c r="D27" s="36">
+        <v>0</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>48</v>
+      </c>
       <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -11020,11 +11055,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11032,11 +11067,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>2 h 10 min</v>
+        <v>2 h 40 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.16352201257861634</v>
+        <v>0.17486338797814208</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11057,11 +11092,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>535</v>
+        <v>565</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11069,11 +11104,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>8 h 55 min</v>
+        <v>9 h 25 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.67295597484276726</v>
+        <v>0.61748633879781423</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11127,7 +11162,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
@@ -11135,7 +11170,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11143,11 +11178,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 10 min</v>
+        <v>3 h 10 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.16352201257861634</v>
+        <v>0.20765027322404372</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11199,26 +11234,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>795</v>
+        <v>915</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>13 h 15 min</v>
+        <v>15 h 15 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.14722222222222223</v>
+        <v>0.16944444444444445</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11262,20 +11297,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8ff2034f-5386-4151-8c46-54da7a5b32f0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8ff2034f-5386-4151-8c46-54da7a5b32f0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11467,14 +11502,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="8ff2034f-5386-4151-8c46-54da7a5b32f0"/>
@@ -11486,6 +11513,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>